<commit_message>
morning 2 march 17
</commit_message>
<xml_diff>
--- a/Jupyter/simulationID/cim_0315_1240/agents.xlsx
+++ b/Jupyter/simulationID/cim_0315_1240/agents.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10203"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shai/Google Drive/BatYam NY DRIVE/Simulations/March 14 GitHUB/BatYamNY/Jupyter/simulationID/cim_0315_1240/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3C4FB3-C3BD-3D41-84CF-2CD425E162AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="34100" yWindow="-2680" windowWidth="31960" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$259</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -148,8 +157,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +221,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -258,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,9 +307,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,6 +359,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,14 +552,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -579,7 +634,7 @@
         <v>1179442.2</v>
       </c>
       <c r="G2">
-        <v>4339.7504</v>
+        <v>4339.7503999999999</v>
       </c>
       <c r="H2">
         <v>91</v>
@@ -615,7 +670,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -635,7 +690,7 @@
         <v>181293.3</v>
       </c>
       <c r="G3">
-        <v>4437.8504</v>
+        <v>4437.8504000000003</v>
       </c>
       <c r="H3">
         <v>86</v>
@@ -671,7 +726,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -691,7 +746,7 @@
         <v>1358903.1</v>
       </c>
       <c r="G4">
-        <v>4825.1504</v>
+        <v>4825.1504000000004</v>
       </c>
       <c r="H4">
         <v>80</v>
@@ -727,7 +782,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -747,7 +802,7 @@
         <v>1377466.2</v>
       </c>
       <c r="G5">
-        <v>1594.7504</v>
+        <v>1594.7503999999999</v>
       </c>
       <c r="H5">
         <v>60</v>
@@ -783,7 +838,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -803,7 +858,7 @@
         <v>93061.8</v>
       </c>
       <c r="G6">
-        <v>7236.1504</v>
+        <v>7236.1504000000004</v>
       </c>
       <c r="H6">
         <v>105</v>
@@ -839,7 +894,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -856,10 +911,10 @@
         <v>2219886</v>
       </c>
       <c r="F7">
-        <v>665965.7999999999</v>
+        <v>665965.79999999993</v>
       </c>
       <c r="G7">
-        <v>4508.0504</v>
+        <v>4508.0504000000001</v>
       </c>
       <c r="H7">
         <v>77</v>
@@ -895,7 +950,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -915,7 +970,7 @@
         <v>1168957.5</v>
       </c>
       <c r="G8">
-        <v>2438.0504</v>
+        <v>2438.0504000000001</v>
       </c>
       <c r="H8">
         <v>32</v>
@@ -951,7 +1006,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -971,7 +1026,7 @@
         <v>1352719.5</v>
       </c>
       <c r="G9">
-        <v>6800.8504</v>
+        <v>6800.8504000000003</v>
       </c>
       <c r="H9">
         <v>98</v>
@@ -1007,7 +1062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1063,7 +1118,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1083,7 +1138,7 @@
         <v>575907.6</v>
       </c>
       <c r="G11">
-        <v>7195.3504</v>
+        <v>7195.3504000000003</v>
       </c>
       <c r="H11">
         <v>36</v>
@@ -1119,7 +1174,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1139,7 +1194,7 @@
         <v>1215572.7</v>
       </c>
       <c r="G12">
-        <v>1737.2504</v>
+        <v>1737.2503999999999</v>
       </c>
       <c r="H12">
         <v>103</v>
@@ -1175,7 +1230,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1195,7 +1250,7 @@
         <v>487083.9</v>
       </c>
       <c r="G13">
-        <v>3965.3504</v>
+        <v>3965.3503999999998</v>
       </c>
       <c r="H13">
         <v>74</v>
@@ -1231,7 +1286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1251,7 +1306,7 @@
         <v>28492.2</v>
       </c>
       <c r="G14">
-        <v>6205.6504</v>
+        <v>6205.6504000000004</v>
       </c>
       <c r="H14">
         <v>106</v>
@@ -1287,7 +1342,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1307,7 +1362,7 @@
         <v>258666.6</v>
       </c>
       <c r="G15">
-        <v>3521.0504</v>
+        <v>3521.0504000000001</v>
       </c>
       <c r="H15">
         <v>92</v>
@@ -1343,7 +1398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1360,10 +1415,10 @@
         <v>3499288</v>
       </c>
       <c r="F16">
-        <v>1049786.4</v>
+        <v>1049786.3999999999</v>
       </c>
       <c r="G16">
-        <v>6442.9504</v>
+        <v>6442.9503999999997</v>
       </c>
       <c r="H16">
         <v>47</v>
@@ -1399,7 +1454,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1416,10 +1471,10 @@
         <v>98952</v>
       </c>
       <c r="F17">
-        <v>29685.6</v>
+        <v>29685.599999999999</v>
       </c>
       <c r="G17">
-        <v>6062.8504</v>
+        <v>6062.8504000000003</v>
       </c>
       <c r="H17">
         <v>41</v>
@@ -1455,7 +1510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1472,7 +1527,7 @@
         <v>1077087</v>
       </c>
       <c r="F18">
-        <v>323126.1</v>
+        <v>323126.09999999998</v>
       </c>
       <c r="G18">
         <v>3134.6504</v>
@@ -1511,7 +1566,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1531,7 +1586,7 @@
         <v>130109.1</v>
       </c>
       <c r="G19">
-        <v>6911.2504</v>
+        <v>6911.2503999999999</v>
       </c>
       <c r="H19">
         <v>65</v>
@@ -1567,7 +1622,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1623,7 +1678,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1643,7 +1698,7 @@
         <v>293061.3</v>
       </c>
       <c r="G21">
-        <v>5004.679999999999</v>
+        <v>5004.6799999999994</v>
       </c>
       <c r="H21">
         <v>28</v>
@@ -1679,7 +1734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1696,7 +1751,7 @@
         <v>1766569</v>
       </c>
       <c r="F22">
-        <v>529970.7</v>
+        <v>529970.69999999995</v>
       </c>
       <c r="G22">
         <v>4796.78</v>
@@ -1735,7 +1790,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1791,7 +1846,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1811,7 +1866,7 @@
         <v>1342642.2</v>
       </c>
       <c r="G24">
-        <v>8215.780000000001</v>
+        <v>8215.7800000000007</v>
       </c>
       <c r="H24">
         <v>29</v>
@@ -1847,7 +1902,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1903,7 +1958,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1959,7 +2014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2015,7 +2070,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2071,7 +2126,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2127,7 +2182,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2144,10 +2199,10 @@
         <v>114856</v>
       </c>
       <c r="F30">
-        <v>34456.8</v>
+        <v>34456.800000000003</v>
       </c>
       <c r="G30">
-        <v>4431.98</v>
+        <v>4431.9799999999996</v>
       </c>
       <c r="H30">
         <v>50</v>
@@ -2183,7 +2238,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2239,7 +2294,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2259,7 +2314,7 @@
         <v>50785.2</v>
       </c>
       <c r="G32">
-        <v>7449.565199999999</v>
+        <v>7449.5651999999991</v>
       </c>
       <c r="H32">
         <v>35</v>
@@ -2295,7 +2350,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2315,7 +2370,7 @@
         <v>231356.7</v>
       </c>
       <c r="G33">
-        <v>7279.4652</v>
+        <v>7279.4651999999996</v>
       </c>
       <c r="H33">
         <v>26</v>
@@ -2351,7 +2406,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2371,7 +2426,7 @@
         <v>1025992.8</v>
       </c>
       <c r="G34">
-        <v>7706.365199999999</v>
+        <v>7706.3651999999993</v>
       </c>
       <c r="H34">
         <v>65</v>
@@ -2407,7 +2462,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2424,10 +2479,10 @@
         <v>17332</v>
       </c>
       <c r="F35">
-        <v>5199.599999999999</v>
+        <v>5199.5999999999995</v>
       </c>
       <c r="G35">
-        <v>7076.065199999999</v>
+        <v>7076.0651999999991</v>
       </c>
       <c r="H35">
         <v>43</v>
@@ -2463,7 +2518,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2519,7 +2574,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2536,10 +2591,10 @@
         <v>305428</v>
       </c>
       <c r="F37">
-        <v>91628.39999999999</v>
+        <v>91628.4</v>
       </c>
       <c r="G37">
-        <v>7990.765199999999</v>
+        <v>7990.7651999999989</v>
       </c>
       <c r="H37">
         <v>37</v>
@@ -2575,7 +2630,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2595,7 +2650,7 @@
         <v>906065.7</v>
       </c>
       <c r="G38">
-        <v>3354.4652</v>
+        <v>3354.4652000000001</v>
       </c>
       <c r="H38">
         <v>96</v>
@@ -2631,7 +2686,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2651,7 +2706,7 @@
         <v>286048.2</v>
       </c>
       <c r="G39">
-        <v>7754.065199999999</v>
+        <v>7754.0651999999991</v>
       </c>
       <c r="H39">
         <v>96</v>
@@ -2687,7 +2742,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2707,7 +2762,7 @@
         <v>1322285.7</v>
       </c>
       <c r="G40">
-        <v>7679.365199999999</v>
+        <v>7679.3651999999993</v>
       </c>
       <c r="H40">
         <v>109</v>
@@ -2743,7 +2798,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2763,7 +2818,7 @@
         <v>1108828.2</v>
       </c>
       <c r="G41">
-        <v>7241.665199999999</v>
+        <v>7241.6651999999985</v>
       </c>
       <c r="H41">
         <v>72</v>
@@ -2799,7 +2854,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2819,7 +2874,7 @@
         <v>258647.7</v>
       </c>
       <c r="G42">
-        <v>7399.765199999999</v>
+        <v>7399.7651999999989</v>
       </c>
       <c r="H42">
         <v>61</v>
@@ -2855,7 +2910,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2872,10 +2927,10 @@
         <v>4239678</v>
       </c>
       <c r="F43">
-        <v>1271903.4</v>
+        <v>1271903.3999999999</v>
       </c>
       <c r="G43">
-        <v>7484.665199999999</v>
+        <v>7484.6651999999985</v>
       </c>
       <c r="H43">
         <v>75</v>
@@ -2911,7 +2966,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2931,7 +2986,7 @@
         <v>1418056.8</v>
       </c>
       <c r="G44">
-        <v>4671.985</v>
+        <v>4671.9849999999997</v>
       </c>
       <c r="H44">
         <v>93</v>
@@ -2967,7 +3022,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2987,7 +3042,7 @@
         <v>552355.5</v>
       </c>
       <c r="G45">
-        <v>5473.285000000001</v>
+        <v>5473.2850000000008</v>
       </c>
       <c r="H45">
         <v>26</v>
@@ -3023,7 +3078,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3043,7 +3098,7 @@
         <v>1074884.7</v>
       </c>
       <c r="G46">
-        <v>4126.884999999999</v>
+        <v>4126.8849999999993</v>
       </c>
       <c r="H46">
         <v>32</v>
@@ -3079,7 +3134,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3096,10 +3151,10 @@
         <v>1863634</v>
       </c>
       <c r="F47">
-        <v>559090.2</v>
+        <v>559090.19999999995</v>
       </c>
       <c r="G47">
-        <v>2732.785</v>
+        <v>2732.7849999999999</v>
       </c>
       <c r="H47">
         <v>30</v>
@@ -3135,7 +3190,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3191,7 +3246,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3208,7 +3263,7 @@
         <v>129261</v>
       </c>
       <c r="F49">
-        <v>38778.3</v>
+        <v>38778.300000000003</v>
       </c>
       <c r="G49">
         <v>3787.585</v>
@@ -3247,7 +3302,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3264,7 +3319,7 @@
         <v>2864336</v>
       </c>
       <c r="F50">
-        <v>859300.7999999999</v>
+        <v>859300.79999999993</v>
       </c>
       <c r="G50">
         <v>3770.184999999999</v>
@@ -3303,7 +3358,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3323,7 +3378,7 @@
         <v>1346985.9</v>
       </c>
       <c r="G51">
-        <v>6025.285000000001</v>
+        <v>6025.2850000000008</v>
       </c>
       <c r="H51">
         <v>84</v>
@@ -3359,7 +3414,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3415,7 +3470,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3471,7 +3526,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3491,7 +3546,7 @@
         <v>486652.2</v>
       </c>
       <c r="G54">
-        <v>4811.785</v>
+        <v>4811.7849999999999</v>
       </c>
       <c r="H54">
         <v>102</v>
@@ -3527,7 +3582,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3547,7 +3602,7 @@
         <v>1078161.3</v>
       </c>
       <c r="G55">
-        <v>3269.785</v>
+        <v>3269.7849999999999</v>
       </c>
       <c r="H55">
         <v>45</v>
@@ -3583,7 +3638,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3639,7 +3694,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3659,7 +3714,7 @@
         <v>363869.4</v>
       </c>
       <c r="G57">
-        <v>1413.685</v>
+        <v>1413.6849999999999</v>
       </c>
       <c r="H57">
         <v>97</v>
@@ -3695,7 +3750,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3712,7 +3767,7 @@
         <v>4473162</v>
       </c>
       <c r="F58">
-        <v>1341948.6</v>
+        <v>1341948.6000000001</v>
       </c>
       <c r="G58">
         <v>4258.585</v>
@@ -3751,7 +3806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3771,7 +3826,7 @@
         <v>1292102.7</v>
       </c>
       <c r="G59">
-        <v>5794.885000000001</v>
+        <v>5794.8850000000011</v>
       </c>
       <c r="H59">
         <v>89</v>
@@ -3807,7 +3862,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3827,7 +3882,7 @@
         <v>653921.1</v>
       </c>
       <c r="G60">
-        <v>2669.185</v>
+        <v>2669.1849999999999</v>
       </c>
       <c r="H60">
         <v>48</v>
@@ -3863,7 +3918,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3883,7 +3938,7 @@
         <v>119488.2</v>
       </c>
       <c r="G61">
-        <v>4663.884999999999</v>
+        <v>4663.8849999999993</v>
       </c>
       <c r="H61">
         <v>104</v>
@@ -3919,7 +3974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3939,7 +3994,7 @@
         <v>1061674.8</v>
       </c>
       <c r="G62">
-        <v>2850.564</v>
+        <v>2850.5639999999999</v>
       </c>
       <c r="H62">
         <v>99</v>
@@ -3975,7 +4030,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3995,7 +4050,7 @@
         <v>1418990.1</v>
       </c>
       <c r="G63">
-        <v>6701.964</v>
+        <v>6701.9639999999999</v>
       </c>
       <c r="H63">
         <v>96</v>
@@ -4031,7 +4086,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4048,10 +4103,10 @@
         <v>1799979</v>
       </c>
       <c r="F64">
-        <v>539993.7</v>
+        <v>539993.69999999995</v>
       </c>
       <c r="G64">
-        <v>5763.864</v>
+        <v>5763.8639999999996</v>
       </c>
       <c r="H64">
         <v>51</v>
@@ -4087,7 +4142,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4107,7 +4162,7 @@
         <v>1394100.9</v>
       </c>
       <c r="G65">
-        <v>1542.264</v>
+        <v>1542.2639999999999</v>
       </c>
       <c r="H65">
         <v>47</v>
@@ -4143,7 +4198,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4163,7 +4218,7 @@
         <v>1485133.2</v>
       </c>
       <c r="G66">
-        <v>3547.464</v>
+        <v>3547.4639999999999</v>
       </c>
       <c r="H66">
         <v>43</v>
@@ -4199,7 +4254,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4216,10 +4271,10 @@
         <v>3563278</v>
       </c>
       <c r="F67">
-        <v>1068983.4</v>
+        <v>1068983.3999999999</v>
       </c>
       <c r="G67">
-        <v>6102.564</v>
+        <v>6102.5640000000003</v>
       </c>
       <c r="H67">
         <v>82</v>
@@ -4255,7 +4310,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4275,7 +4330,7 @@
         <v>825894</v>
       </c>
       <c r="G68">
-        <v>6150.864</v>
+        <v>6150.8639999999996</v>
       </c>
       <c r="H68">
         <v>66</v>
@@ -4311,7 +4366,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4328,10 +4383,10 @@
         <v>2117799</v>
       </c>
       <c r="F69">
-        <v>635339.7</v>
+        <v>635339.69999999995</v>
       </c>
       <c r="G69">
-        <v>3121.464</v>
+        <v>3121.4639999999999</v>
       </c>
       <c r="H69">
         <v>97</v>
@@ -4367,7 +4422,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4387,7 +4442,7 @@
         <v>1381416</v>
       </c>
       <c r="G70">
-        <v>4247.364</v>
+        <v>4247.3639999999996</v>
       </c>
       <c r="H70">
         <v>52</v>
@@ -4423,7 +4478,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4443,7 +4498,7 @@
         <v>1377383.4</v>
       </c>
       <c r="G71">
-        <v>2248.464</v>
+        <v>2248.4639999999999</v>
       </c>
       <c r="H71">
         <v>45</v>
@@ -4479,7 +4534,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4499,7 +4554,7 @@
         <v>1457233.8</v>
       </c>
       <c r="G72">
-        <v>5372.964</v>
+        <v>5372.9639999999999</v>
       </c>
       <c r="H72">
         <v>83</v>
@@ -4535,7 +4590,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4555,7 +4610,7 @@
         <v>1055915.7</v>
       </c>
       <c r="G73">
-        <v>5783.064</v>
+        <v>5783.0640000000003</v>
       </c>
       <c r="H73">
         <v>79</v>
@@ -4591,7 +4646,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4611,7 +4666,7 @@
         <v>870120.9</v>
       </c>
       <c r="G74">
-        <v>4974.4652</v>
+        <v>4974.4651999999996</v>
       </c>
       <c r="H74">
         <v>87</v>
@@ -4647,7 +4702,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4703,7 +4758,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4723,7 +4778,7 @@
         <v>544140.6</v>
       </c>
       <c r="G76">
-        <v>5068.9652</v>
+        <v>5068.9651999999996</v>
       </c>
       <c r="H76">
         <v>47</v>
@@ -4759,7 +4814,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4776,7 +4831,7 @@
         <v>2666881</v>
       </c>
       <c r="F77">
-        <v>800064.2999999999</v>
+        <v>800064.29999999993</v>
       </c>
       <c r="G77">
         <v>4522.0652</v>
@@ -4815,7 +4870,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4835,7 +4890,7 @@
         <v>1410715.5</v>
       </c>
       <c r="G78">
-        <v>2057.2652</v>
+        <v>2057.2651999999998</v>
       </c>
       <c r="H78">
         <v>106</v>
@@ -4871,7 +4926,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4888,7 +4943,7 @@
         <v>4319793</v>
       </c>
       <c r="F79">
-        <v>1295937.9</v>
+        <v>1295937.8999999999</v>
       </c>
       <c r="G79">
         <v>4783.0652</v>
@@ -4927,7 +4982,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4947,7 +5002,7 @@
         <v>1093339.8</v>
       </c>
       <c r="G80">
-        <v>6825.985000000001</v>
+        <v>6825.9850000000006</v>
       </c>
       <c r="H80">
         <v>48</v>
@@ -4983,7 +5038,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5039,7 +5094,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5059,7 +5114,7 @@
         <v>1365671.7</v>
       </c>
       <c r="G82">
-        <v>2304.685</v>
+        <v>2304.6849999999999</v>
       </c>
       <c r="H82">
         <v>85</v>
@@ -5095,7 +5150,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5112,10 +5167,10 @@
         <v>1752281</v>
       </c>
       <c r="F83">
-        <v>525684.2999999999</v>
+        <v>525684.29999999993</v>
       </c>
       <c r="G83">
-        <v>1888.285</v>
+        <v>1888.2850000000001</v>
       </c>
       <c r="H83">
         <v>73</v>
@@ -5151,7 +5206,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -5171,7 +5226,7 @@
         <v>504919.8</v>
       </c>
       <c r="G84">
-        <v>2400.385</v>
+        <v>2400.3850000000002</v>
       </c>
       <c r="H84">
         <v>49</v>
@@ -5207,7 +5262,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -5224,7 +5279,7 @@
         <v>2025239</v>
       </c>
       <c r="F85">
-        <v>607571.7</v>
+        <v>607571.69999999995</v>
       </c>
       <c r="G85">
         <v>3426.085</v>
@@ -5263,7 +5318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5283,7 +5338,7 @@
         <v>744704.4</v>
       </c>
       <c r="G86">
-        <v>2354.785</v>
+        <v>2354.7849999999999</v>
       </c>
       <c r="H86">
         <v>31</v>
@@ -5319,7 +5374,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5336,10 +5391,10 @@
         <v>2195244</v>
       </c>
       <c r="F87">
-        <v>658573.2</v>
+        <v>658573.19999999995</v>
       </c>
       <c r="G87">
-        <v>2168.785</v>
+        <v>2168.7849999999999</v>
       </c>
       <c r="H87">
         <v>41</v>
@@ -5375,7 +5430,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5392,10 +5447,10 @@
         <v>2180599</v>
       </c>
       <c r="F88">
-        <v>654179.7</v>
+        <v>654179.69999999995</v>
       </c>
       <c r="G88">
-        <v>1804.285</v>
+        <v>1804.2850000000001</v>
       </c>
       <c r="H88">
         <v>91</v>
@@ -5431,7 +5486,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5451,7 +5506,7 @@
         <v>1454116.8</v>
       </c>
       <c r="G89">
-        <v>2325.985</v>
+        <v>2325.9850000000001</v>
       </c>
       <c r="H89">
         <v>39</v>
@@ -5487,7 +5542,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5507,7 +5562,7 @@
         <v>713413.5</v>
       </c>
       <c r="G90">
-        <v>7170.685</v>
+        <v>7170.6850000000004</v>
       </c>
       <c r="H90">
         <v>39</v>
@@ -5543,7 +5598,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -5599,7 +5654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -5619,7 +5674,7 @@
         <v>1472710.2</v>
       </c>
       <c r="G92">
-        <v>4673.785</v>
+        <v>4673.7849999999999</v>
       </c>
       <c r="H92">
         <v>83</v>
@@ -5655,7 +5710,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -5675,7 +5730,7 @@
         <v>1028677.5</v>
       </c>
       <c r="G93">
-        <v>4761.684999999999</v>
+        <v>4761.6849999999986</v>
       </c>
       <c r="H93">
         <v>80</v>
@@ -5711,7 +5766,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -5731,7 +5786,7 @@
         <v>661125.9</v>
       </c>
       <c r="G94">
-        <v>6356.185</v>
+        <v>6356.1850000000004</v>
       </c>
       <c r="H94">
         <v>101</v>
@@ -5767,7 +5822,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -5787,7 +5842,7 @@
         <v>720239.7</v>
       </c>
       <c r="G95">
-        <v>1902.685</v>
+        <v>1902.6849999999999</v>
       </c>
       <c r="H95">
         <v>69</v>
@@ -5823,7 +5878,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -5879,7 +5934,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -5899,7 +5954,7 @@
         <v>1088221.2</v>
       </c>
       <c r="G97">
-        <v>1904.485</v>
+        <v>1904.4849999999999</v>
       </c>
       <c r="H97">
         <v>36</v>
@@ -5935,7 +5990,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -5955,7 +6010,7 @@
         <v>344818.5</v>
       </c>
       <c r="G98">
-        <v>4827.684999999999</v>
+        <v>4827.6849999999986</v>
       </c>
       <c r="H98">
         <v>60</v>
@@ -5991,7 +6046,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -6008,10 +6063,10 @@
         <v>1041932</v>
       </c>
       <c r="F99">
-        <v>312579.6</v>
+        <v>312579.59999999998</v>
       </c>
       <c r="G99">
-        <v>3143.185</v>
+        <v>3143.1849999999999</v>
       </c>
       <c r="H99">
         <v>108</v>
@@ -6047,7 +6102,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -6067,7 +6122,7 @@
         <v>672186.9</v>
       </c>
       <c r="G100">
-        <v>1476.985</v>
+        <v>1476.9849999999999</v>
       </c>
       <c r="H100">
         <v>26</v>
@@ -6103,7 +6158,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6159,7 +6214,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -6179,7 +6234,7 @@
         <v>1376055</v>
       </c>
       <c r="G102">
-        <v>3368.785</v>
+        <v>3368.7849999999999</v>
       </c>
       <c r="H102">
         <v>50</v>
@@ -6215,7 +6270,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -6232,7 +6287,7 @@
         <v>3770408</v>
       </c>
       <c r="F103">
-        <v>1131122.4</v>
+        <v>1131122.3999999999</v>
       </c>
       <c r="G103">
         <v>3850.585</v>
@@ -6271,7 +6326,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -6291,7 +6346,7 @@
         <v>1342517.1</v>
       </c>
       <c r="G104">
-        <v>4971.384999999999</v>
+        <v>4971.3849999999993</v>
       </c>
       <c r="H104">
         <v>54</v>
@@ -6327,7 +6382,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -6383,7 +6438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -6403,7 +6458,7 @@
         <v>916789.2</v>
       </c>
       <c r="G106">
-        <v>3501.685</v>
+        <v>3501.6849999999999</v>
       </c>
       <c r="H106">
         <v>51</v>
@@ -6439,7 +6494,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -6456,10 +6511,10 @@
         <v>4455162</v>
       </c>
       <c r="F107">
-        <v>1336548.6</v>
+        <v>1336548.6000000001</v>
       </c>
       <c r="G107">
-        <v>2613.685</v>
+        <v>2613.6849999999999</v>
       </c>
       <c r="H107">
         <v>56</v>
@@ -6495,7 +6550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -6551,7 +6606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -6607,7 +6662,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -6627,7 +6682,7 @@
         <v>779345.7</v>
       </c>
       <c r="G110">
-        <v>4536.684999999999</v>
+        <v>4536.6849999999986</v>
       </c>
       <c r="H110">
         <v>42</v>
@@ -6663,7 +6718,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -6683,7 +6738,7 @@
         <v>1355698.2</v>
       </c>
       <c r="G111">
-        <v>4486.285</v>
+        <v>4486.2849999999999</v>
       </c>
       <c r="H111">
         <v>84</v>
@@ -6719,7 +6774,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -6739,7 +6794,7 @@
         <v>1355208.6</v>
       </c>
       <c r="G112">
-        <v>3135.385</v>
+        <v>3135.3850000000002</v>
       </c>
       <c r="H112">
         <v>77</v>
@@ -6775,7 +6830,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="113" spans="1:18">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -6792,10 +6847,10 @@
         <v>248007</v>
       </c>
       <c r="F113">
-        <v>74402.09999999999</v>
+        <v>74402.099999999991</v>
       </c>
       <c r="G113">
-        <v>3671.185</v>
+        <v>3671.1849999999999</v>
       </c>
       <c r="H113">
         <v>96</v>
@@ -6831,7 +6886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="1:18">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -6851,7 +6906,7 @@
         <v>452682</v>
       </c>
       <c r="G114">
-        <v>4837.884999999999</v>
+        <v>4837.8849999999993</v>
       </c>
       <c r="H114">
         <v>84</v>
@@ -6887,7 +6942,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -6907,7 +6962,7 @@
         <v>951660.6</v>
       </c>
       <c r="G115">
-        <v>2400.385</v>
+        <v>2400.3850000000002</v>
       </c>
       <c r="H115">
         <v>53</v>
@@ -6943,7 +6998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="1:18">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -6963,7 +7018,7 @@
         <v>1449272.1</v>
       </c>
       <c r="G116">
-        <v>4961.785</v>
+        <v>4961.7849999999999</v>
       </c>
       <c r="H116">
         <v>59</v>
@@ -6999,7 +7054,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="117" spans="1:18">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -7019,7 +7074,7 @@
         <v>500121.9</v>
       </c>
       <c r="G117">
-        <v>2526.985</v>
+        <v>2526.9850000000001</v>
       </c>
       <c r="H117">
         <v>37</v>
@@ -7055,7 +7110,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="118" spans="1:18">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -7072,10 +7127,10 @@
         <v>2155091</v>
       </c>
       <c r="F118">
-        <v>646527.2999999999</v>
+        <v>646527.29999999993</v>
       </c>
       <c r="G118">
-        <v>6543.685</v>
+        <v>6543.6850000000004</v>
       </c>
       <c r="H118">
         <v>63</v>
@@ -7111,7 +7166,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="1:18">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -7128,10 +7183,10 @@
         <v>286823</v>
       </c>
       <c r="F119">
-        <v>86046.89999999999</v>
+        <v>86046.9</v>
       </c>
       <c r="G119">
-        <v>4629.384999999999</v>
+        <v>4629.3849999999993</v>
       </c>
       <c r="H119">
         <v>43</v>
@@ -7167,7 +7222,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -7187,7 +7242,7 @@
         <v>127660.5</v>
       </c>
       <c r="G120">
-        <v>6286.543</v>
+        <v>6286.5429999999997</v>
       </c>
       <c r="H120">
         <v>51</v>
@@ -7223,7 +7278,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="121" spans="1:18">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -7240,7 +7295,7 @@
         <v>2328016</v>
       </c>
       <c r="F121">
-        <v>698404.7999999999</v>
+        <v>698404.79999999993</v>
       </c>
       <c r="G121">
         <v>1492.943</v>
@@ -7279,7 +7334,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="122" spans="1:18">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -7299,7 +7354,7 @@
         <v>558693</v>
       </c>
       <c r="G122">
-        <v>4963.343</v>
+        <v>4963.3429999999998</v>
       </c>
       <c r="H122">
         <v>70</v>
@@ -7335,7 +7390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="123" spans="1:18">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -7355,7 +7410,7 @@
         <v>1222568.7</v>
       </c>
       <c r="G123">
-        <v>7209.043</v>
+        <v>7209.0429999999997</v>
       </c>
       <c r="H123">
         <v>53</v>
@@ -7391,7 +7446,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="124" spans="1:18">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -7411,7 +7466,7 @@
         <v>740717.4</v>
       </c>
       <c r="G124">
-        <v>7204.242999999999</v>
+        <v>7204.2429999999986</v>
       </c>
       <c r="H124">
         <v>107</v>
@@ -7447,7 +7502,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="125" spans="1:18">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -7467,7 +7522,7 @@
         <v>894371.4</v>
       </c>
       <c r="G125">
-        <v>2006.843</v>
+        <v>2006.8430000000001</v>
       </c>
       <c r="H125">
         <v>45</v>
@@ -7503,7 +7558,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="126" spans="1:18">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -7520,10 +7575,10 @@
         <v>3550507</v>
       </c>
       <c r="F126">
-        <v>1065152.1</v>
+        <v>1065152.1000000001</v>
       </c>
       <c r="G126">
-        <v>2287.343</v>
+        <v>2287.3429999999998</v>
       </c>
       <c r="H126">
         <v>83</v>
@@ -7559,7 +7614,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="127" spans="1:18">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -7579,7 +7634,7 @@
         <v>880392.6</v>
       </c>
       <c r="G127">
-        <v>2330.243</v>
+        <v>2330.2429999999999</v>
       </c>
       <c r="H127">
         <v>101</v>
@@ -7615,7 +7670,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -7635,7 +7690,7 @@
         <v>1112362.8</v>
       </c>
       <c r="G128">
-        <v>3196.343</v>
+        <v>3196.3429999999998</v>
       </c>
       <c r="H128">
         <v>52</v>
@@ -7671,7 +7726,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:18">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -7691,7 +7746,7 @@
         <v>1010170.8</v>
       </c>
       <c r="G129">
-        <v>4708.343</v>
+        <v>4708.3429999999998</v>
       </c>
       <c r="H129">
         <v>58</v>
@@ -7727,7 +7782,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="130" spans="1:18">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -7747,7 +7802,7 @@
         <v>518109</v>
       </c>
       <c r="G130">
-        <v>6456.343</v>
+        <v>6456.3429999999998</v>
       </c>
       <c r="H130">
         <v>46</v>
@@ -7783,7 +7838,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:18">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -7800,10 +7855,10 @@
         <v>4431332</v>
       </c>
       <c r="F131">
-        <v>1329399.6</v>
+        <v>1329399.6000000001</v>
       </c>
       <c r="G131">
-        <v>6800.443</v>
+        <v>6800.4430000000002</v>
       </c>
       <c r="H131">
         <v>50</v>
@@ -7839,7 +7894,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:18">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -7895,7 +7950,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -7951,7 +8006,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="134" spans="1:18">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -7971,7 +8026,7 @@
         <v>410601.6</v>
       </c>
       <c r="G134">
-        <v>6432.343</v>
+        <v>6432.3429999999998</v>
       </c>
       <c r="H134">
         <v>99</v>
@@ -8007,7 +8062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="135" spans="1:18">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -8024,7 +8079,7 @@
         <v>1851586</v>
       </c>
       <c r="F135">
-        <v>555475.7999999999</v>
+        <v>555475.79999999993</v>
       </c>
       <c r="G135">
         <v>6074.143</v>
@@ -8063,7 +8118,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="136" spans="1:18">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -8083,7 +8138,7 @@
         <v>570423.9</v>
       </c>
       <c r="G136">
-        <v>2337.743</v>
+        <v>2337.7429999999999</v>
       </c>
       <c r="H136">
         <v>104</v>
@@ -8119,7 +8174,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="137" spans="1:18">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -8139,7 +8194,7 @@
         <v>917160</v>
       </c>
       <c r="G137">
-        <v>3479.243</v>
+        <v>3479.2429999999999</v>
       </c>
       <c r="H137">
         <v>63</v>
@@ -8175,7 +8230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="138" spans="1:18">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -8192,7 +8247,7 @@
         <v>2795916</v>
       </c>
       <c r="F138">
-        <v>838774.7999999999</v>
+        <v>838774.79999999993</v>
       </c>
       <c r="G138">
         <v>3745.643</v>
@@ -8231,7 +8286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="139" spans="1:18">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -8251,7 +8306,7 @@
         <v>321246</v>
       </c>
       <c r="G139">
-        <v>2231.843</v>
+        <v>2231.8429999999998</v>
       </c>
       <c r="H139">
         <v>57</v>
@@ -8287,7 +8342,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="140" spans="1:18">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -8307,7 +8362,7 @@
         <v>18618</v>
       </c>
       <c r="G140">
-        <v>4813.943</v>
+        <v>4813.9430000000002</v>
       </c>
       <c r="H140">
         <v>109</v>
@@ -8343,7 +8398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="141" spans="1:18">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -8360,10 +8415,10 @@
         <v>1798874</v>
       </c>
       <c r="F141">
-        <v>539662.2</v>
+        <v>539662.19999999995</v>
       </c>
       <c r="G141">
-        <v>3931.943</v>
+        <v>3931.9430000000002</v>
       </c>
       <c r="H141">
         <v>36</v>
@@ -8399,7 +8454,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -8416,10 +8471,10 @@
         <v>1768376</v>
       </c>
       <c r="F142">
-        <v>530512.7999999999</v>
+        <v>530512.79999999993</v>
       </c>
       <c r="G142">
-        <v>6477.043</v>
+        <v>6477.0429999999997</v>
       </c>
       <c r="H142">
         <v>35</v>
@@ -8455,7 +8510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:18">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -8511,7 +8566,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="144" spans="1:18">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -8567,7 +8622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="145" spans="1:18">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -8587,7 +8642,7 @@
         <v>865006.2</v>
       </c>
       <c r="G145">
-        <v>2753.427</v>
+        <v>2753.4270000000001</v>
       </c>
       <c r="H145">
         <v>109</v>
@@ -8623,7 +8678,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="146" spans="1:18">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -8679,7 +8734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="147" spans="1:18">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -8699,7 +8754,7 @@
         <v>948214.5</v>
       </c>
       <c r="G147">
-        <v>4613.727</v>
+        <v>4613.7269999999999</v>
       </c>
       <c r="H147">
         <v>96</v>
@@ -8735,7 +8790,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="148" spans="1:18">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -8752,7 +8807,7 @@
         <v>2604906</v>
       </c>
       <c r="F148">
-        <v>781471.7999999999</v>
+        <v>781471.79999999993</v>
       </c>
       <c r="G148">
         <v>1839.027</v>
@@ -8791,7 +8846,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="149" spans="1:18">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -8811,7 +8866,7 @@
         <v>781623.6</v>
       </c>
       <c r="G149">
-        <v>1708.227</v>
+        <v>1708.2270000000001</v>
       </c>
       <c r="H149">
         <v>103</v>
@@ -8847,7 +8902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="150" spans="1:18">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -8867,7 +8922,7 @@
         <v>294440.7</v>
       </c>
       <c r="G150">
-        <v>1988.427</v>
+        <v>1988.4269999999999</v>
       </c>
       <c r="H150">
         <v>69</v>
@@ -8903,7 +8958,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="151" spans="1:18">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -8920,7 +8975,7 @@
         <v>242247</v>
       </c>
       <c r="F151">
-        <v>72674.09999999999</v>
+        <v>72674.099999999991</v>
       </c>
       <c r="G151">
         <v>2100.627</v>
@@ -8959,7 +9014,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="152" spans="1:18">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -8979,7 +9034,7 @@
         <v>1225064.7</v>
       </c>
       <c r="G152">
-        <v>4741.827</v>
+        <v>4741.8270000000002</v>
       </c>
       <c r="H152">
         <v>75</v>
@@ -9015,7 +9070,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="153" spans="1:18">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -9071,7 +9126,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="154" spans="1:18">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -9088,10 +9143,10 @@
         <v>2665936</v>
       </c>
       <c r="F154">
-        <v>799780.7999999999</v>
+        <v>799780.79999999993</v>
       </c>
       <c r="G154">
-        <v>2057.243</v>
+        <v>2057.2429999999999</v>
       </c>
       <c r="H154">
         <v>38</v>
@@ -9127,7 +9182,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="155" spans="1:18">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -9147,7 +9202,7 @@
         <v>1463123.4</v>
       </c>
       <c r="G155">
-        <v>6471.943</v>
+        <v>6471.9430000000002</v>
       </c>
       <c r="H155">
         <v>54</v>
@@ -9183,7 +9238,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="156" spans="1:18">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -9200,10 +9255,10 @@
         <v>1035257</v>
       </c>
       <c r="F156">
-        <v>310577.1</v>
+        <v>310577.09999999998</v>
       </c>
       <c r="G156">
-        <v>6918.943</v>
+        <v>6918.9430000000002</v>
       </c>
       <c r="H156">
         <v>39</v>
@@ -9239,7 +9294,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="157" spans="1:18">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -9259,7 +9314,7 @@
         <v>1019622</v>
       </c>
       <c r="G157">
-        <v>4941.742999999999</v>
+        <v>4941.7429999999986</v>
       </c>
       <c r="H157">
         <v>61</v>
@@ -9295,7 +9350,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="158" spans="1:18">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -9312,10 +9367,10 @@
         <v>3528048</v>
       </c>
       <c r="F158">
-        <v>1058414.4</v>
+        <v>1058414.3999999999</v>
       </c>
       <c r="G158">
-        <v>1574.543</v>
+        <v>1574.5429999999999</v>
       </c>
       <c r="H158">
         <v>58</v>
@@ -9351,7 +9406,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="159" spans="1:18">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -9371,7 +9426,7 @@
         <v>782600.1</v>
       </c>
       <c r="G159">
-        <v>6825.343</v>
+        <v>6825.3429999999998</v>
       </c>
       <c r="H159">
         <v>52</v>
@@ -9407,7 +9462,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="160" spans="1:18">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -9424,10 +9479,10 @@
         <v>2228651</v>
       </c>
       <c r="F160">
-        <v>668595.2999999999</v>
+        <v>668595.29999999993</v>
       </c>
       <c r="G160">
-        <v>3872.543</v>
+        <v>3872.5430000000001</v>
       </c>
       <c r="H160">
         <v>35</v>
@@ -9463,7 +9518,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="161" spans="1:18">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -9483,7 +9538,7 @@
         <v>1491762.6</v>
       </c>
       <c r="G161">
-        <v>4699.043</v>
+        <v>4699.0429999999997</v>
       </c>
       <c r="H161">
         <v>68</v>
@@ -9519,7 +9574,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="162" spans="1:18">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -9539,7 +9594,7 @@
         <v>691722</v>
       </c>
       <c r="G162">
-        <v>4750.043</v>
+        <v>4750.0429999999997</v>
       </c>
       <c r="H162">
         <v>99</v>
@@ -9575,7 +9630,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" spans="1:18">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -9592,10 +9647,10 @@
         <v>176136</v>
       </c>
       <c r="F163">
-        <v>52840.8</v>
+        <v>52840.800000000003</v>
       </c>
       <c r="G163">
-        <v>7390.543</v>
+        <v>7390.5429999999997</v>
       </c>
       <c r="H163">
         <v>67</v>
@@ -9631,7 +9686,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="164" spans="1:18">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -9648,10 +9703,10 @@
         <v>3295211</v>
       </c>
       <c r="F164">
-        <v>988563.2999999999</v>
+        <v>988563.29999999993</v>
       </c>
       <c r="G164">
-        <v>2533.943</v>
+        <v>2533.9430000000002</v>
       </c>
       <c r="H164">
         <v>36</v>
@@ -9687,7 +9742,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="165" spans="1:18">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -9707,7 +9762,7 @@
         <v>353273.1</v>
       </c>
       <c r="G165">
-        <v>4557.443</v>
+        <v>4557.4430000000002</v>
       </c>
       <c r="H165">
         <v>55</v>
@@ -9743,7 +9798,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="166" spans="1:18">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -9763,7 +9818,7 @@
         <v>1470648.9</v>
       </c>
       <c r="G166">
-        <v>2228.2924</v>
+        <v>2228.2923999999998</v>
       </c>
       <c r="H166">
         <v>70</v>
@@ -9799,7 +9854,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="167" spans="1:18">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -9819,7 +9874,7 @@
         <v>623503.5</v>
       </c>
       <c r="G167">
-        <v>6732.792399999999</v>
+        <v>6732.7923999999994</v>
       </c>
       <c r="H167">
         <v>25</v>
@@ -9855,7 +9910,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="168" spans="1:18">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -9872,7 +9927,7 @@
         <v>4326887</v>
       </c>
       <c r="F168">
-        <v>1298066.1</v>
+        <v>1298066.1000000001</v>
       </c>
       <c r="G168">
         <v>2611.0924</v>
@@ -9911,7 +9966,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="169" spans="1:18">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -9931,7 +9986,7 @@
         <v>816418.5</v>
       </c>
       <c r="G169">
-        <v>2892.7924</v>
+        <v>2892.7923999999998</v>
       </c>
       <c r="H169">
         <v>54</v>
@@ -9967,7 +10022,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="170" spans="1:18">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -9984,10 +10039,10 @@
         <v>2090971</v>
       </c>
       <c r="F170">
-        <v>627291.2999999999</v>
+        <v>627291.29999999993</v>
       </c>
       <c r="G170">
-        <v>2537.2924</v>
+        <v>2537.2923999999998</v>
       </c>
       <c r="H170">
         <v>64</v>
@@ -10023,7 +10078,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="171" spans="1:18">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -10040,10 +10095,10 @@
         <v>68903</v>
       </c>
       <c r="F171">
-        <v>20670.9</v>
+        <v>20670.900000000001</v>
       </c>
       <c r="G171">
-        <v>4697.8924</v>
+        <v>4697.8923999999997</v>
       </c>
       <c r="H171">
         <v>43</v>
@@ -10079,7 +10134,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="172" spans="1:18">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -10099,7 +10154,7 @@
         <v>128845.8</v>
       </c>
       <c r="G172">
-        <v>3513.7924</v>
+        <v>3513.7923999999998</v>
       </c>
       <c r="H172">
         <v>87</v>
@@ -10135,7 +10190,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="173" spans="1:18">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -10152,10 +10207,10 @@
         <v>1937839</v>
       </c>
       <c r="F173">
-        <v>581351.7</v>
+        <v>581351.69999999995</v>
       </c>
       <c r="G173">
-        <v>1602.4924</v>
+        <v>1602.4924000000001</v>
       </c>
       <c r="H173">
         <v>95</v>
@@ -10191,7 +10246,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="174" spans="1:18">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -10211,7 +10266,7 @@
         <v>274135.2</v>
       </c>
       <c r="G174">
-        <v>6184.3924</v>
+        <v>6184.3923999999997</v>
       </c>
       <c r="H174">
         <v>28</v>
@@ -10247,7 +10302,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="175" spans="1:18">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -10303,7 +10358,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="176" spans="1:18">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -10323,7 +10378,7 @@
         <v>1484626.2</v>
       </c>
       <c r="G176">
-        <v>4294.9924</v>
+        <v>4294.9924000000001</v>
       </c>
       <c r="H176">
         <v>67</v>
@@ -10359,7 +10414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="177" spans="1:18">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -10379,7 +10434,7 @@
         <v>675209.1</v>
       </c>
       <c r="G177">
-        <v>5515.3924</v>
+        <v>5515.3923999999997</v>
       </c>
       <c r="H177">
         <v>97</v>
@@ -10415,7 +10470,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="178" spans="1:18">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -10435,7 +10490,7 @@
         <v>911607.6</v>
       </c>
       <c r="G178">
-        <v>4256.8924</v>
+        <v>4256.8923999999997</v>
       </c>
       <c r="H178">
         <v>47</v>
@@ -10471,7 +10526,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="179" spans="1:18">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -10491,7 +10546,7 @@
         <v>52378.2</v>
       </c>
       <c r="G179">
-        <v>3643.3924</v>
+        <v>3643.3924000000002</v>
       </c>
       <c r="H179">
         <v>54</v>
@@ -10527,7 +10582,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="180" spans="1:18">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -10547,7 +10602,7 @@
         <v>108419.7</v>
       </c>
       <c r="G180">
-        <v>1804.9924</v>
+        <v>1804.9924000000001</v>
       </c>
       <c r="H180">
         <v>32</v>
@@ -10583,7 +10638,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="181" spans="1:18">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -10600,10 +10655,10 @@
         <v>54948</v>
       </c>
       <c r="F181">
-        <v>16484.4</v>
+        <v>16484.400000000001</v>
       </c>
       <c r="G181">
-        <v>6259.0924</v>
+        <v>6259.0924000000005</v>
       </c>
       <c r="H181">
         <v>95</v>
@@ -10639,7 +10694,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="182" spans="1:18">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -10656,10 +10711,10 @@
         <v>3672423</v>
       </c>
       <c r="F182">
-        <v>1101726.9</v>
+        <v>1101726.8999999999</v>
       </c>
       <c r="G182">
-        <v>2480.2924</v>
+        <v>2480.2923999999998</v>
       </c>
       <c r="H182">
         <v>63</v>
@@ -10695,7 +10750,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="183" spans="1:18">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -10715,7 +10770,7 @@
         <v>359939.4</v>
       </c>
       <c r="G183">
-        <v>5914.6924</v>
+        <v>5914.6923999999999</v>
       </c>
       <c r="H183">
         <v>39</v>
@@ -10751,7 +10806,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="184" spans="1:18">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -10771,7 +10826,7 @@
         <v>1172946.3</v>
       </c>
       <c r="G184">
-        <v>6385.971399999999</v>
+        <v>6385.9713999999994</v>
       </c>
       <c r="H184">
         <v>46</v>
@@ -10807,7 +10862,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="185" spans="1:18">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -10824,10 +10879,10 @@
         <v>984052</v>
       </c>
       <c r="F185">
-        <v>295215.6</v>
+        <v>295215.59999999998</v>
       </c>
       <c r="G185">
-        <v>5192.2714</v>
+        <v>5192.2713999999996</v>
       </c>
       <c r="H185">
         <v>61</v>
@@ -10863,7 +10918,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="186" spans="1:18">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -10919,7 +10974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="187" spans="1:18">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -10939,7 +10994,7 @@
         <v>1021346.4</v>
       </c>
       <c r="G187">
-        <v>2579.4714</v>
+        <v>2579.4713999999999</v>
       </c>
       <c r="H187">
         <v>33</v>
@@ -10975,7 +11030,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="188" spans="1:18">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -10995,7 +11050,7 @@
         <v>1169812.2</v>
       </c>
       <c r="G188">
-        <v>5560.0714</v>
+        <v>5560.0713999999998</v>
       </c>
       <c r="H188">
         <v>61</v>
@@ -11031,7 +11086,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="189" spans="1:18">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -11048,7 +11103,7 @@
         <v>905747</v>
       </c>
       <c r="F189">
-        <v>271724.1</v>
+        <v>271724.09999999998</v>
       </c>
       <c r="G189">
         <v>1749.3714</v>
@@ -11087,7 +11142,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="190" spans="1:18">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -11107,7 +11162,7 @@
         <v>822260.7</v>
       </c>
       <c r="G190">
-        <v>6213.471399999999</v>
+        <v>6213.4713999999994</v>
       </c>
       <c r="H190">
         <v>57</v>
@@ -11143,7 +11198,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="191" spans="1:18">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -11163,7 +11218,7 @@
         <v>1019923.5</v>
       </c>
       <c r="G191">
-        <v>3200.1714</v>
+        <v>3200.1714000000002</v>
       </c>
       <c r="H191">
         <v>67</v>
@@ -11199,7 +11254,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="192" spans="1:18">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -11216,10 +11271,10 @@
         <v>920708</v>
       </c>
       <c r="F192">
-        <v>276212.4</v>
+        <v>276212.40000000002</v>
       </c>
       <c r="G192">
-        <v>5850.7714</v>
+        <v>5850.7713999999996</v>
       </c>
       <c r="H192">
         <v>86</v>
@@ -11255,7 +11310,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="193" spans="1:18">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -11275,7 +11330,7 @@
         <v>1277088.3</v>
       </c>
       <c r="G193">
-        <v>4849.5714</v>
+        <v>4849.5713999999998</v>
       </c>
       <c r="H193">
         <v>74</v>
@@ -11311,7 +11366,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="194" spans="1:18">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -11331,7 +11386,7 @@
         <v>708237.9</v>
       </c>
       <c r="G194">
-        <v>1610.7714</v>
+        <v>1610.7714000000001</v>
       </c>
       <c r="H194">
         <v>35</v>
@@ -11367,7 +11422,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="195" spans="1:18">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -11387,7 +11442,7 @@
         <v>588585</v>
       </c>
       <c r="G195">
-        <v>3907.2714</v>
+        <v>3907.2714000000001</v>
       </c>
       <c r="H195">
         <v>54</v>
@@ -11423,7 +11478,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="196" spans="1:18">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -11479,7 +11534,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="197" spans="1:18">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -11499,7 +11554,7 @@
         <v>689272.5</v>
       </c>
       <c r="G197">
-        <v>5821.6714</v>
+        <v>5821.6714000000002</v>
       </c>
       <c r="H197">
         <v>47</v>
@@ -11535,7 +11590,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="198" spans="1:18">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -11552,10 +11607,10 @@
         <v>208513</v>
       </c>
       <c r="F198">
-        <v>62553.89999999999</v>
+        <v>62553.899999999987</v>
       </c>
       <c r="G198">
-        <v>5696.5714</v>
+        <v>5696.5713999999998</v>
       </c>
       <c r="H198">
         <v>48</v>
@@ -11591,7 +11646,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="199" spans="1:18">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -11647,7 +11702,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="200" spans="1:18">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -11703,7 +11758,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="201" spans="1:18">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -11720,7 +11775,7 @@
         <v>4316203</v>
       </c>
       <c r="F201">
-        <v>1294860.9</v>
+        <v>1294860.8999999999</v>
       </c>
       <c r="G201">
         <v>5006.8714</v>
@@ -11759,7 +11814,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="202" spans="1:18">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -11779,7 +11834,7 @@
         <v>574251</v>
       </c>
       <c r="G202">
-        <v>3596.7492</v>
+        <v>3596.7492000000002</v>
       </c>
       <c r="H202">
         <v>59</v>
@@ -11815,7 +11870,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="203" spans="1:18">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -11835,7 +11890,7 @@
         <v>770102.4</v>
       </c>
       <c r="G203">
-        <v>6538.649200000001</v>
+        <v>6538.6492000000007</v>
       </c>
       <c r="H203">
         <v>93</v>
@@ -11871,7 +11926,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="204" spans="1:18">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -11888,7 +11943,7 @@
         <v>2002046</v>
       </c>
       <c r="F204">
-        <v>600613.7999999999</v>
+        <v>600613.79999999993</v>
       </c>
       <c r="G204">
         <v>2033.4492</v>
@@ -11927,7 +11982,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="205" spans="1:18">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -11947,7 +12002,7 @@
         <v>129651.9</v>
       </c>
       <c r="G205">
-        <v>2467.8492</v>
+        <v>2467.8492000000001</v>
       </c>
       <c r="H205">
         <v>25</v>
@@ -11983,7 +12038,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="206" spans="1:18">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -12003,7 +12058,7 @@
         <v>702032.1</v>
       </c>
       <c r="G206">
-        <v>6590.849200000001</v>
+        <v>6590.8492000000006</v>
       </c>
       <c r="H206">
         <v>109</v>
@@ -12039,7 +12094,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="207" spans="1:18">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -12056,7 +12111,7 @@
         <v>885242</v>
       </c>
       <c r="F207">
-        <v>265572.6</v>
+        <v>265572.59999999998</v>
       </c>
       <c r="G207">
         <v>4208.4492</v>
@@ -12095,7 +12150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="208" spans="1:18">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -12112,7 +12167,7 @@
         <v>2686726</v>
       </c>
       <c r="F208">
-        <v>806017.7999999999</v>
+        <v>806017.79999999993</v>
       </c>
       <c r="G208">
         <v>2313.9492</v>
@@ -12151,7 +12206,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="209" spans="1:18">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -12171,7 +12226,7 @@
         <v>788115.6</v>
       </c>
       <c r="G209">
-        <v>3799.5492</v>
+        <v>3799.5491999999999</v>
       </c>
       <c r="H209">
         <v>26</v>
@@ -12207,7 +12262,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="210" spans="1:18">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -12224,10 +12279,10 @@
         <v>4131423</v>
       </c>
       <c r="F210">
-        <v>1239426.9</v>
+        <v>1239426.8999999999</v>
       </c>
       <c r="G210">
-        <v>3975.3492</v>
+        <v>3975.3492000000001</v>
       </c>
       <c r="H210">
         <v>49</v>
@@ -12263,7 +12318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="211" spans="1:18">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -12283,7 +12338,7 @@
         <v>650976</v>
       </c>
       <c r="G211">
-        <v>6121.0492</v>
+        <v>6121.0492000000004</v>
       </c>
       <c r="H211">
         <v>85</v>
@@ -12319,7 +12374,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="212" spans="1:18">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -12339,7 +12394,7 @@
         <v>123925.2</v>
       </c>
       <c r="G212">
-        <v>1601.1492</v>
+        <v>1601.1492000000001</v>
       </c>
       <c r="H212">
         <v>53</v>
@@ -12375,7 +12430,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="213" spans="1:18">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -12395,7 +12450,7 @@
         <v>1437435.3</v>
       </c>
       <c r="G213">
-        <v>5998.349200000001</v>
+        <v>5998.3492000000006</v>
       </c>
       <c r="H213">
         <v>79</v>
@@ -12431,7 +12486,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="214" spans="1:18">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -12451,7 +12506,7 @@
         <v>794471.1</v>
       </c>
       <c r="G214">
-        <v>3609.6492</v>
+        <v>3609.6491999999998</v>
       </c>
       <c r="H214">
         <v>74</v>
@@ -12487,7 +12542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="215" spans="1:18">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -12507,7 +12562,7 @@
         <v>465162.6</v>
       </c>
       <c r="G215">
-        <v>4375.5492</v>
+        <v>4375.5492000000004</v>
       </c>
       <c r="H215">
         <v>39</v>
@@ -12543,7 +12598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="216" spans="1:18">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -12563,7 +12618,7 @@
         <v>1456150.2</v>
       </c>
       <c r="G216">
-        <v>5675.5492</v>
+        <v>5675.5492000000004</v>
       </c>
       <c r="H216">
         <v>86</v>
@@ -12599,7 +12654,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="217" spans="1:18">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -12619,7 +12674,7 @@
         <v>792473.1</v>
       </c>
       <c r="G217">
-        <v>3820.5492</v>
+        <v>3820.5491999999999</v>
       </c>
       <c r="H217">
         <v>90</v>
@@ -12655,7 +12710,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="218" spans="1:18">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -12711,7 +12766,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="219" spans="1:18">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -12731,7 +12786,7 @@
         <v>69687.3</v>
       </c>
       <c r="G219">
-        <v>6097.349200000001</v>
+        <v>6097.3492000000006</v>
       </c>
       <c r="H219">
         <v>27</v>
@@ -12767,7 +12822,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="220" spans="1:18">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -12787,7 +12842,7 @@
         <v>519392.4</v>
       </c>
       <c r="G220">
-        <v>2737.4998</v>
+        <v>2737.4998000000001</v>
       </c>
       <c r="H220">
         <v>93</v>
@@ -12823,7 +12878,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="221" spans="1:18">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -12843,7 +12898,7 @@
         <v>1270651.5</v>
       </c>
       <c r="G221">
-        <v>3271.1998</v>
+        <v>3271.1997999999999</v>
       </c>
       <c r="H221">
         <v>76</v>
@@ -12879,7 +12934,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="222" spans="1:18">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -12935,7 +12990,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="223" spans="1:18">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -12952,7 +13007,7 @@
         <v>1846769</v>
       </c>
       <c r="F223">
-        <v>554030.7</v>
+        <v>554030.69999999995</v>
       </c>
       <c r="G223">
         <v>3207.5998</v>
@@ -12991,7 +13046,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="224" spans="1:18">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -13011,7 +13066,7 @@
         <v>1377715.8</v>
       </c>
       <c r="G224">
-        <v>1448.6998</v>
+        <v>1448.6998000000001</v>
       </c>
       <c r="H224">
         <v>28</v>
@@ -13047,7 +13102,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="225" spans="1:18">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -13067,7 +13122,7 @@
         <v>45936.3</v>
       </c>
       <c r="G225">
-        <v>3567.2998</v>
+        <v>3567.2997999999998</v>
       </c>
       <c r="H225">
         <v>36</v>
@@ -13103,7 +13158,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="226" spans="1:18">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -13159,7 +13214,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="227" spans="1:18">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -13179,7 +13234,7 @@
         <v>838842</v>
       </c>
       <c r="G227">
-        <v>4006.4998</v>
+        <v>4006.4998000000001</v>
       </c>
       <c r="H227">
         <v>105</v>
@@ -13215,7 +13270,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="228" spans="1:18">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -13232,10 +13287,10 @@
         <v>3774873</v>
       </c>
       <c r="F228">
-        <v>1132461.9</v>
+        <v>1132461.8999999999</v>
       </c>
       <c r="G228">
-        <v>4454.699799999999</v>
+        <v>4454.6997999999994</v>
       </c>
       <c r="H228">
         <v>87</v>
@@ -13271,7 +13326,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="229" spans="1:18">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -13291,7 +13346,7 @@
         <v>1346563.8</v>
       </c>
       <c r="G229">
-        <v>2519.9998</v>
+        <v>2519.9998000000001</v>
       </c>
       <c r="H229">
         <v>45</v>
@@ -13327,7 +13382,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="230" spans="1:18">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -13347,7 +13402,7 @@
         <v>260010</v>
       </c>
       <c r="G230">
-        <v>3056.9998</v>
+        <v>3056.9998000000001</v>
       </c>
       <c r="H230">
         <v>25</v>
@@ -13383,7 +13438,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="231" spans="1:18">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -13403,7 +13458,7 @@
         <v>960259.2</v>
       </c>
       <c r="G231">
-        <v>2401.7998</v>
+        <v>2401.7997999999998</v>
       </c>
       <c r="H231">
         <v>27</v>
@@ -13439,7 +13494,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="232" spans="1:18">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -13459,7 +13514,7 @@
         <v>511505.7</v>
       </c>
       <c r="G232">
-        <v>2256.2998</v>
+        <v>2256.2997999999998</v>
       </c>
       <c r="H232">
         <v>65</v>
@@ -13495,7 +13550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="233" spans="1:18">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -13515,7 +13570,7 @@
         <v>802118.4</v>
       </c>
       <c r="G233">
-        <v>3806.9998</v>
+        <v>3806.9998000000001</v>
       </c>
       <c r="H233">
         <v>102</v>
@@ -13551,7 +13606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="234" spans="1:18">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -13568,10 +13623,10 @@
         <v>2592016</v>
       </c>
       <c r="F234">
-        <v>777604.7999999999</v>
+        <v>777604.79999999993</v>
       </c>
       <c r="G234">
-        <v>1802.6998</v>
+        <v>1802.6998000000001</v>
       </c>
       <c r="H234">
         <v>36</v>
@@ -13607,7 +13662,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="235" spans="1:18">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -13627,7 +13682,7 @@
         <v>246966.6</v>
       </c>
       <c r="G235">
-        <v>4648.199799999999</v>
+        <v>4648.1997999999994</v>
       </c>
       <c r="H235">
         <v>69</v>
@@ -13663,7 +13718,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="236" spans="1:18">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -13683,7 +13738,7 @@
         <v>191868</v>
       </c>
       <c r="G236">
-        <v>3297.264</v>
+        <v>3297.2640000000001</v>
       </c>
       <c r="H236">
         <v>26</v>
@@ -13719,7 +13774,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="237" spans="1:18">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -13739,7 +13794,7 @@
         <v>1467079.8</v>
       </c>
       <c r="G237">
-        <v>2437.164</v>
+        <v>2437.1640000000002</v>
       </c>
       <c r="H237">
         <v>77</v>
@@ -13775,7 +13830,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="238" spans="1:18">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -13792,10 +13847,10 @@
         <v>2439721</v>
       </c>
       <c r="F238">
-        <v>731916.2999999999</v>
+        <v>731916.29999999993</v>
       </c>
       <c r="G238">
-        <v>2754.264</v>
+        <v>2754.2640000000001</v>
       </c>
       <c r="H238">
         <v>81</v>
@@ -13831,7 +13886,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="239" spans="1:18">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -13887,7 +13942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="240" spans="1:18">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -13907,7 +13962,7 @@
         <v>1461997.2</v>
       </c>
       <c r="G240">
-        <v>6064.563999999999</v>
+        <v>6064.5639999999994</v>
       </c>
       <c r="H240">
         <v>49</v>
@@ -13943,7 +13998,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="241" spans="1:18">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -13963,7 +14018,7 @@
         <v>906138</v>
       </c>
       <c r="G241">
-        <v>6934.264</v>
+        <v>6934.2640000000001</v>
       </c>
       <c r="H241">
         <v>61</v>
@@ -13999,7 +14054,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="242" spans="1:18">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -14016,10 +14071,10 @@
         <v>3888102</v>
       </c>
       <c r="F242">
-        <v>1166430.6</v>
+        <v>1166430.6000000001</v>
       </c>
       <c r="G242">
-        <v>5759.764</v>
+        <v>5759.7640000000001</v>
       </c>
       <c r="H242">
         <v>66</v>
@@ -14055,7 +14110,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="243" spans="1:18">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -14075,7 +14130,7 @@
         <v>345991.2</v>
       </c>
       <c r="G243">
-        <v>6413.164</v>
+        <v>6413.1639999999998</v>
       </c>
       <c r="H243">
         <v>29</v>
@@ -14111,7 +14166,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="244" spans="1:18">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -14131,7 +14186,7 @@
         <v>710471.4</v>
       </c>
       <c r="G244">
-        <v>2194.464</v>
+        <v>2194.4639999999999</v>
       </c>
       <c r="H244">
         <v>80</v>
@@ -14167,7 +14222,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="245" spans="1:18">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -14184,10 +14239,10 @@
         <v>2680391</v>
       </c>
       <c r="F245">
-        <v>804117.2999999999</v>
+        <v>804117.29999999993</v>
       </c>
       <c r="G245">
-        <v>6981.364</v>
+        <v>6981.3639999999996</v>
       </c>
       <c r="H245">
         <v>77</v>
@@ -14223,7 +14278,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="246" spans="1:18">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -14279,7 +14334,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="247" spans="1:18">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -14335,7 +14390,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="248" spans="1:18">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -14355,7 +14410,7 @@
         <v>202971.3</v>
       </c>
       <c r="G248">
-        <v>6285.964</v>
+        <v>6285.9639999999999</v>
       </c>
       <c r="H248">
         <v>97</v>
@@ -14391,7 +14446,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="249" spans="1:18">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -14411,7 +14466,7 @@
         <v>194260.2</v>
       </c>
       <c r="G249">
-        <v>6246.964</v>
+        <v>6246.9639999999999</v>
       </c>
       <c r="H249">
         <v>46</v>
@@ -14447,7 +14502,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="250" spans="1:18">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -14503,7 +14558,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="251" spans="1:18">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -14520,10 +14575,10 @@
         <v>3153313</v>
       </c>
       <c r="F251">
-        <v>945993.8999999999</v>
+        <v>945993.89999999991</v>
       </c>
       <c r="G251">
-        <v>4828.164</v>
+        <v>4828.1639999999998</v>
       </c>
       <c r="H251">
         <v>46</v>
@@ -14559,7 +14614,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="252" spans="1:18">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -14579,7 +14634,7 @@
         <v>904463.7</v>
       </c>
       <c r="G252">
-        <v>6358.563999999999</v>
+        <v>6358.5639999999994</v>
       </c>
       <c r="H252">
         <v>74</v>
@@ -14615,7 +14670,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="253" spans="1:18">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -14671,7 +14726,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="254" spans="1:18">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -14688,10 +14743,10 @@
         <v>1932246</v>
       </c>
       <c r="F254">
-        <v>579673.7999999999</v>
+        <v>579673.79999999993</v>
       </c>
       <c r="G254">
-        <v>5800.264</v>
+        <v>5800.2640000000001</v>
       </c>
       <c r="H254">
         <v>88</v>
@@ -14727,7 +14782,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="255" spans="1:18">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -14747,7 +14802,7 @@
         <v>668926.5</v>
       </c>
       <c r="G255">
-        <v>4844.964</v>
+        <v>4844.9639999999999</v>
       </c>
       <c r="H255">
         <v>64</v>
@@ -14783,7 +14838,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="256" spans="1:18">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -14803,7 +14858,7 @@
         <v>660081.6</v>
       </c>
       <c r="G256">
-        <v>6188.464</v>
+        <v>6188.4639999999999</v>
       </c>
       <c r="H256">
         <v>39</v>
@@ -14839,7 +14894,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="257" spans="1:18">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -14859,7 +14914,7 @@
         <v>1289223.3</v>
       </c>
       <c r="G257">
-        <v>4481.664</v>
+        <v>4481.6639999999998</v>
       </c>
       <c r="H257">
         <v>68</v>
@@ -14895,7 +14950,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="258" spans="1:18">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -14912,10 +14967,10 @@
         <v>3189406</v>
       </c>
       <c r="F258">
-        <v>956821.7999999999</v>
+        <v>956821.79999999993</v>
       </c>
       <c r="G258">
-        <v>6805.264</v>
+        <v>6805.2640000000001</v>
       </c>
       <c r="H258">
         <v>41</v>
@@ -14951,7 +15006,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="259" spans="1:18">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -14971,7 +15026,7 @@
         <v>1380542.4</v>
       </c>
       <c r="G259">
-        <v>4230.864</v>
+        <v>4230.8639999999996</v>
       </c>
       <c r="H259">
         <v>101</v>
@@ -15008,6 +15063,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R259" xr:uid="{8BA99CF8-B14F-DF4B-89B0-B543C985AAD6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>